<commit_message>
updated with today's cell
</commit_message>
<xml_diff>
--- a/mouseInfo.xlsx
+++ b/mouseInfo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="99">
   <si>
     <t>Rpip</t>
   </si>
@@ -315,6 +315,15 @@
   </si>
   <si>
     <t>2017.02.24</t>
+  </si>
+  <si>
+    <t>2017.02.28</t>
+  </si>
+  <si>
+    <t>w100</t>
+  </si>
+  <si>
+    <t>2017.03.01</t>
   </si>
 </sst>
 </file>
@@ -914,11 +923,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2936,7 +2945,119 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H53" s="1"/>
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="C53" s="2">
+        <v>42787</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>6.61</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+      <c r="I53" s="1">
+        <v>1.66</v>
+      </c>
+      <c r="J53" t="s">
+        <v>12</v>
+      </c>
+      <c r="K53">
+        <v>61.95</v>
+      </c>
+      <c r="L53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54">
+        <v>15</v>
+      </c>
+      <c r="C54" s="2">
+        <v>42787</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>6.61</v>
+      </c>
+      <c r="H54" s="1">
+        <v>2</v>
+      </c>
+      <c r="I54" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="J54" t="s">
+        <v>97</v>
+      </c>
+      <c r="K54">
+        <v>114.6</v>
+      </c>
+      <c r="L54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55">
+        <v>15</v>
+      </c>
+      <c r="C55" s="2">
+        <v>42788</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>5.86</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+      <c r="I55" s="1">
+        <v>1.47</v>
+      </c>
+      <c r="J55" t="s">
+        <v>10</v>
+      </c>
+      <c r="K55">
+        <v>99.65</v>
+      </c>
+      <c r="L55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
filtering traces by min response capacitance peak
</commit_message>
<xml_diff>
--- a/mouseInfo.xlsx
+++ b/mouseInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuwenwu/ephysAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/lab_data_2/Storage/Ephys/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="150">
   <si>
     <t>Rpip</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>w394</t>
+  </si>
+  <si>
+    <t>2016.09.16</t>
   </si>
 </sst>
 </file>
@@ -1080,11 +1083,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L105" sqref="L105"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,42 +1138,39 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="B2">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>7.11</v>
+        <v>5.4</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1.8</v>
+        <v>1.87</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
       </c>
       <c r="K2">
-        <v>54.57</v>
+        <v>61.39</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>88</v>
@@ -1179,39 +1179,39 @@
         <v>1</v>
       </c>
       <c r="G3">
+        <v>7.11</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1.8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>54.57</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>7.39</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1.7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3">
-        <v>85.95</v>
-      </c>
-      <c r="L3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>6.65</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1220,21 +1220,21 @@
         <v>1.7</v>
       </c>
       <c r="J4" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="K4">
-        <v>79.95</v>
+        <v>85.95</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>86</v>
+      <c r="A5" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>47</v>
@@ -1243,22 +1243,22 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>7.32</v>
+        <v>6.65</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1.55</v>
+        <v>1.7</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
       <c r="K5">
-        <v>92.92</v>
+        <v>79.95</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1272,94 +1272,94 @@
         <v>47</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>7.32</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1.75</v>
+        <v>1.55</v>
       </c>
       <c r="J6" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="K6">
-        <v>95.5</v>
+        <v>92.92</v>
       </c>
       <c r="L6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1.75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7">
+        <v>95.5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>7.82</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>1.77</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>114.6</v>
-      </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2">
-        <v>42661</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>5.68</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1.6</v>
       </c>
       <c r="J8" t="s">
         <v>10</v>
       </c>
       <c r="K8">
-        <v>63.08</v>
+        <v>114.6</v>
+      </c>
+      <c r="L8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -1374,22 +1374,19 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>5.57</v>
+        <v>5.68</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>1.76</v>
+        <v>1.6</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K9">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="L9" t="s">
-        <v>13</v>
+        <v>63.08</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1412,22 +1409,19 @@
         <v>5.57</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1.45</v>
+        <v>1.76</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K10">
-        <v>70.16</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="L10" t="s">
         <v>13</v>
-      </c>
-      <c r="M10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1450,57 +1444,57 @@
         <v>5.57</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>1.55</v>
+        <v>1.45</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K11">
-        <v>61.39</v>
+        <v>70.16</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
       </c>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
         <v>42661</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>10.91</v>
+        <v>5.57</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>1.8</v>
+        <v>1.55</v>
       </c>
       <c r="J12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K12">
-        <v>84.89</v>
+        <v>61.39</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1526,16 +1520,16 @@
         <v>10.91</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K13">
-        <v>76.400000000000006</v>
+        <v>84.89</v>
       </c>
       <c r="L13" t="s">
         <v>19</v>
@@ -1543,43 +1537,40 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2">
-        <v>42668</v>
+        <v>42661</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>6.66</v>
+        <v>10.91</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14">
-        <v>1.67</v>
+        <v>1.9</v>
       </c>
       <c r="J14" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K14">
-        <v>89.3</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="L14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1605,27 +1596,27 @@
         <v>6.66</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="K15">
-        <v>59.79</v>
+        <v>89.3</v>
       </c>
       <c r="L15" t="s">
         <v>22</v>
       </c>
       <c r="M15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1634,34 +1625,34 @@
         <v>42668</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>7.08</v>
+        <v>6.66</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="J16" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="K16">
-        <v>83.85</v>
+        <v>59.79</v>
       </c>
       <c r="L16" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="M16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1669,40 +1660,40 @@
         <v>31</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2">
         <v>42668</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="1">
+        <v>48</v>
+      </c>
+      <c r="E17">
         <v>7</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
+      <c r="F17">
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>6.16</v>
+        <v>7.08</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="J17" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="K17">
-        <v>79.95</v>
+        <v>83.85</v>
       </c>
       <c r="L17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1728,22 +1719,22 @@
         <v>6.16</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="J18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K18">
-        <v>78.14</v>
+        <v>79.95</v>
       </c>
       <c r="L18" t="s">
         <v>33</v>
       </c>
       <c r="M18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1763,36 +1754,36 @@
         <v>7</v>
       </c>
       <c r="F19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
         <v>6.16</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>1.93</v>
+        <v>1.8</v>
       </c>
       <c r="J19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K19">
-        <v>58.77</v>
+        <v>78.14</v>
       </c>
       <c r="L19" t="s">
         <v>33</v>
       </c>
       <c r="M19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2">
         <v>42668</v>
@@ -1801,31 +1792,31 @@
         <v>47</v>
       </c>
       <c r="E20" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>6.71</v>
+        <v>6.16</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20">
-        <v>1.54</v>
+        <v>1.93</v>
       </c>
       <c r="J20" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="K20">
-        <v>61.95</v>
+        <v>58.77</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="M20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1851,139 +1842,142 @@
         <v>6.71</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>1.89</v>
+        <v>1.54</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="K21">
-        <v>96.85</v>
+        <v>61.95</v>
       </c>
       <c r="L21" t="s">
         <v>19</v>
       </c>
+      <c r="M21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2">
         <v>42668</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
-      <c r="G22" s="1">
-        <v>9.44</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1.44</v>
+      <c r="G22">
+        <v>6.71</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>1.89</v>
       </c>
       <c r="J22" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="K22">
-        <v>77.260000000000005</v>
+        <v>96.85</v>
       </c>
       <c r="L22" t="s">
-        <v>42</v>
-      </c>
-      <c r="M22" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B23">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2">
-        <v>42675</v>
+        <v>42668</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="G23" s="1">
-        <v>6.06</v>
+        <v>9.44</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
       </c>
       <c r="I23" s="1">
-        <v>1.6</v>
+        <v>1.44</v>
       </c>
       <c r="J23" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="K23">
-        <v>73.150000000000006</v>
+        <v>77.260000000000005</v>
       </c>
       <c r="L23" t="s">
         <v>42</v>
       </c>
       <c r="M23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" s="2">
-        <v>42682</v>
+        <v>42675</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="1">
-        <v>6.62</v>
+        <v>6.06</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
       </c>
       <c r="I24" s="1">
-        <v>1.63</v>
+        <v>1.6</v>
       </c>
       <c r="J24" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="K24">
-        <v>96.85</v>
+        <v>73.150000000000006</v>
       </c>
       <c r="L24" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="M24" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -2009,16 +2003,16 @@
         <v>6.62</v>
       </c>
       <c r="H25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25" s="1">
-        <v>1.6</v>
+        <v>1.63</v>
       </c>
       <c r="J25" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="K25">
-        <v>82.84</v>
+        <v>96.85</v>
       </c>
       <c r="L25" t="s">
         <v>50</v>
@@ -2026,10 +2020,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B26">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2">
         <v>42682</v>
@@ -2038,31 +2032,28 @@
         <v>48</v>
       </c>
       <c r="E26" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="G26" s="1">
-        <v>7.14</v>
+        <v>6.62</v>
       </c>
       <c r="H26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" s="1">
-        <v>1.45</v>
+        <v>1.6</v>
       </c>
       <c r="J26" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="K26">
-        <v>94.19</v>
+        <v>82.84</v>
       </c>
       <c r="L26" t="s">
-        <v>13</v>
-      </c>
-      <c r="M26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -2088,16 +2079,16 @@
         <v>7.14</v>
       </c>
       <c r="H27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1">
-        <v>1.6</v>
+        <v>1.45</v>
       </c>
       <c r="J27" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="K27">
-        <v>79.040000000000006</v>
+        <v>94.19</v>
       </c>
       <c r="L27" t="s">
         <v>13</v>
@@ -2108,81 +2099,81 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28" s="2">
-        <v>42710</v>
+        <v>42682</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
       <c r="G28" s="1">
-        <v>5.34</v>
+        <v>7.14</v>
       </c>
       <c r="H28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28" s="1">
-        <v>1.69</v>
+        <v>1.6</v>
       </c>
       <c r="J28" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="K28">
-        <v>74.739999999999995</v>
+        <v>79.040000000000006</v>
       </c>
       <c r="L28" t="s">
         <v>13</v>
       </c>
+      <c r="M28" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" s="2">
-        <v>42711</v>
+        <v>42710</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E29" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="1">
-        <v>6.51</v>
+        <v>5.34</v>
       </c>
       <c r="H29" s="1">
         <v>1</v>
       </c>
       <c r="I29" s="1">
-        <v>1.52</v>
+        <v>1.69</v>
       </c>
       <c r="J29" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="K29">
-        <v>90.48</v>
+        <v>74.739999999999995</v>
       </c>
       <c r="L29" t="s">
         <v>13</v>
-      </c>
-      <c r="M29" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -2208,16 +2199,16 @@
         <v>6.51</v>
       </c>
       <c r="H30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" s="1">
-        <v>1.37</v>
+        <v>1.52</v>
       </c>
       <c r="J30" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K30">
-        <v>101.1</v>
+        <v>90.48</v>
       </c>
       <c r="L30" t="s">
         <v>13</v>
@@ -2228,43 +2219,43 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2">
-        <v>42717</v>
+        <v>42711</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E31" s="1">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>6.6</v>
+        <v>6</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6.51</v>
       </c>
       <c r="H31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I31" s="1">
-        <v>1.58</v>
+        <v>1.37</v>
       </c>
       <c r="J31" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="K31">
-        <v>79.95</v>
+        <v>101.1</v>
       </c>
       <c r="L31" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="M31" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -2290,16 +2281,16 @@
         <v>6.6</v>
       </c>
       <c r="H32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1">
-        <v>1.77</v>
+        <v>1.58</v>
       </c>
       <c r="J32" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="K32">
-        <v>87.04</v>
+        <v>79.95</v>
       </c>
       <c r="L32" t="s">
         <v>58</v>
@@ -2331,16 +2322,16 @@
         <v>6.6</v>
       </c>
       <c r="H33" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I33" s="1">
-        <v>1.55</v>
+        <v>1.77</v>
       </c>
       <c r="J33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K33">
-        <v>89.3</v>
+        <v>87.04</v>
       </c>
       <c r="L33" t="s">
         <v>58</v>
@@ -2351,40 +2342,40 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B34">
         <v>15</v>
       </c>
       <c r="C34" s="2">
-        <v>42718</v>
+        <v>42717</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E34" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34">
-        <v>6.73</v>
+        <v>6.6</v>
       </c>
       <c r="H34" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34" s="1">
         <v>1.55</v>
       </c>
       <c r="J34" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="K34">
-        <v>77.260000000000005</v>
+        <v>89.3</v>
       </c>
       <c r="L34" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M34" t="s">
         <v>61</v>
@@ -2392,10 +2383,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B35">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2">
         <v>42718</v>
@@ -2404,28 +2395,28 @@
         <v>47</v>
       </c>
       <c r="E35" s="1">
-        <v>5</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1">
-        <v>7.39</v>
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>6.73</v>
       </c>
       <c r="H35" s="1">
         <v>1</v>
       </c>
       <c r="I35" s="1">
-        <v>1.65</v>
+        <v>1.55</v>
       </c>
       <c r="J35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K35">
-        <v>70.89</v>
+        <v>77.260000000000005</v>
       </c>
       <c r="L35" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="M35" t="s">
         <v>61</v>
@@ -2454,19 +2445,22 @@
         <v>7.39</v>
       </c>
       <c r="H36" s="1">
-        <v>2</v>
-      </c>
-      <c r="I36" s="3">
-        <v>1.35</v>
+        <v>1</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1.65</v>
       </c>
       <c r="J36" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="K36">
-        <v>67.48</v>
+        <v>70.89</v>
       </c>
       <c r="L36" t="s">
         <v>19</v>
+      </c>
+      <c r="M36" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -2492,95 +2486,95 @@
         <v>7.39</v>
       </c>
       <c r="H37" s="1">
-        <v>3</v>
-      </c>
-      <c r="I37" s="1">
-        <v>1.6</v>
+        <v>2</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1.35</v>
       </c>
       <c r="J37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K37">
-        <v>102.6</v>
+        <v>67.48</v>
       </c>
       <c r="L37" t="s">
         <v>19</v>
       </c>
-      <c r="M37" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B38">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C38" s="2">
-        <v>42724</v>
+        <v>42718</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E38" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="1">
-        <v>4.8499999999999996</v>
+        <v>7.39</v>
       </c>
       <c r="H38" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I38" s="1">
-        <v>1.49</v>
+        <v>1.6</v>
       </c>
       <c r="J38" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="K38">
-        <v>79.95</v>
+        <v>102.6</v>
       </c>
       <c r="L38" t="s">
-        <v>63</v>
+        <v>19</v>
+      </c>
+      <c r="M38" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C39" s="2">
-        <v>42725</v>
+        <v>42724</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E39" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="1">
-        <v>8.85</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H39" s="1">
         <v>1</v>
       </c>
       <c r="I39" s="1">
-        <v>1.45</v>
+        <v>1.49</v>
       </c>
       <c r="J39" t="s">
         <v>10</v>
       </c>
       <c r="K39">
-        <v>76.400000000000006</v>
+        <v>79.95</v>
       </c>
       <c r="L39" t="s">
         <v>63</v>
@@ -2609,16 +2603,16 @@
         <v>8.85</v>
       </c>
       <c r="H40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I40" s="1">
         <v>1.45</v>
       </c>
       <c r="J40" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K40">
-        <v>69.459999999999994</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="L40" t="s">
         <v>63</v>
@@ -2626,10 +2620,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="2">
         <v>42725</v>
@@ -2638,69 +2632,66 @@
         <v>47</v>
       </c>
       <c r="E41" s="1">
+        <v>3</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>8.85</v>
+      </c>
+      <c r="H41" s="1">
         <v>2</v>
       </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1">
-        <v>9.01</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1</v>
-      </c>
       <c r="I41" s="1">
-        <v>1.4</v>
+        <v>1.45</v>
       </c>
       <c r="J41" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K41">
-        <v>80.900000000000006</v>
+        <v>69.459999999999994</v>
       </c>
       <c r="L41" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B42">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C42" s="2">
-        <v>42760</v>
+        <v>42725</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E42" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="1">
-        <v>5.43</v>
+        <v>9.01</v>
       </c>
       <c r="H42" s="1">
         <v>1</v>
       </c>
       <c r="I42" s="1">
-        <v>1.45</v>
+        <v>1.4</v>
       </c>
       <c r="J42" t="s">
         <v>10</v>
       </c>
       <c r="K42">
-        <v>83.85</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="L42" t="s">
-        <v>13</v>
-      </c>
-      <c r="M42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -2726,22 +2717,22 @@
         <v>5.43</v>
       </c>
       <c r="H43" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" s="1">
-        <v>1.35</v>
+        <v>1.45</v>
       </c>
       <c r="J43" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="K43">
-        <v>74.739999999999995</v>
+        <v>83.85</v>
       </c>
       <c r="L43" t="s">
         <v>13</v>
       </c>
       <c r="M43" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -2767,63 +2758,63 @@
         <v>5.43</v>
       </c>
       <c r="H44" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I44" s="1">
-        <v>1.68</v>
+        <v>1.35</v>
       </c>
       <c r="J44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K44">
-        <v>83.85</v>
+        <v>74.739999999999995</v>
       </c>
       <c r="L44" t="s">
         <v>13</v>
       </c>
       <c r="M44" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B45">
         <v>15</v>
       </c>
       <c r="C45" s="2">
-        <v>42766</v>
+        <v>42760</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E45" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="1">
-        <v>4.3</v>
+        <v>5.43</v>
       </c>
       <c r="H45" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I45" s="1">
-        <v>1.58</v>
+        <v>1.68</v>
       </c>
       <c r="J45" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="K45">
-        <v>63.08</v>
+        <v>83.85</v>
       </c>
       <c r="L45" t="s">
         <v>13</v>
       </c>
       <c r="M45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -2849,22 +2840,22 @@
         <v>4.3</v>
       </c>
       <c r="H46" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I46" s="1">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
       <c r="J46" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="K46">
-        <v>64.87</v>
+        <v>63.08</v>
       </c>
       <c r="L46" t="s">
         <v>13</v>
       </c>
       <c r="M46" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -2890,71 +2881,71 @@
         <v>4.3</v>
       </c>
       <c r="H47" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I47" s="1">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="J47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K47">
-        <v>57.78</v>
+        <v>64.87</v>
       </c>
       <c r="L47" t="s">
-        <v>81</v>
+        <v>13</v>
+      </c>
+      <c r="M47" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B48">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C48" s="2">
-        <v>42767</v>
+        <v>42766</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E48">
-        <v>6</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>7.08</v>
+      <c r="E48" s="1">
+        <v>5</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1">
+        <v>4.3</v>
       </c>
       <c r="H48" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I48" s="1">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="J48" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="K48">
-        <v>69.459999999999994</v>
+        <v>57.78</v>
       </c>
       <c r="L48" t="s">
-        <v>42</v>
-      </c>
-      <c r="M48" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B49">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C49" s="2">
-        <v>42781</v>
+        <v>42767</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>47</v>
@@ -2966,22 +2957,25 @@
         <v>1</v>
       </c>
       <c r="G49">
-        <v>6.04</v>
+        <v>7.08</v>
       </c>
       <c r="H49" s="1">
         <v>1</v>
       </c>
       <c r="I49" s="1">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="J49" t="s">
         <v>10</v>
       </c>
       <c r="K49">
-        <v>68.760000000000005</v>
+        <v>69.459999999999994</v>
       </c>
       <c r="L49" t="s">
-        <v>63</v>
+        <v>42</v>
+      </c>
+      <c r="M49" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -3007,16 +3001,16 @@
         <v>6.04</v>
       </c>
       <c r="H50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" s="1">
-        <v>1.58</v>
+        <v>1.5</v>
       </c>
       <c r="J50" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="K50">
-        <v>82.84</v>
+        <v>68.760000000000005</v>
       </c>
       <c r="L50" t="s">
         <v>63</v>
@@ -3045,16 +3039,16 @@
         <v>6.04</v>
       </c>
       <c r="H51" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I51" s="1">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
       <c r="J51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K51">
-        <v>70.89</v>
+        <v>82.84</v>
       </c>
       <c r="L51" t="s">
         <v>63</v>
@@ -3062,10 +3056,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B52">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C52" s="2">
         <v>42781</v>
@@ -3074,69 +3068,69 @@
         <v>47</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F52">
         <v>1</v>
       </c>
       <c r="G52">
-        <v>6.85</v>
+        <v>6.04</v>
       </c>
       <c r="H52" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I52" s="1">
-        <v>1.65</v>
+        <v>1.6</v>
       </c>
       <c r="J52" t="s">
+        <v>94</v>
+      </c>
+      <c r="K52">
+        <v>70.89</v>
+      </c>
+      <c r="L52" t="s">
         <v>63</v>
-      </c>
-      <c r="K52">
-        <v>78.14</v>
-      </c>
-      <c r="L52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M52" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C53" s="2">
-        <v>42787</v>
+        <v>42781</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E53">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F53">
         <v>1</v>
       </c>
       <c r="G53">
-        <v>6.61</v>
+        <v>6.85</v>
       </c>
       <c r="H53" s="1">
         <v>1</v>
       </c>
       <c r="I53" s="1">
-        <v>1.66</v>
+        <v>1.65</v>
       </c>
       <c r="J53" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="K53">
-        <v>61.95</v>
+        <v>78.14</v>
       </c>
       <c r="L53" t="s">
-        <v>50</v>
+        <v>33</v>
+      </c>
+      <c r="M53" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -3162,16 +3156,16 @@
         <v>6.61</v>
       </c>
       <c r="H54" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54" s="1">
-        <v>1.3</v>
+        <v>1.66</v>
       </c>
       <c r="J54" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="K54">
-        <v>114.6</v>
+        <v>61.95</v>
       </c>
       <c r="L54" t="s">
         <v>50</v>
@@ -3179,48 +3173,48 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B55">
         <v>15</v>
       </c>
       <c r="C55" s="2">
-        <v>42788</v>
+        <v>42787</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55">
-        <v>5.86</v>
+        <v>6.61</v>
       </c>
       <c r="H55" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I55" s="1">
-        <v>1.47</v>
+        <v>1.3</v>
       </c>
       <c r="J55" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="K55">
-        <v>99.65</v>
+        <v>114.6</v>
       </c>
       <c r="L55" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C56" s="2">
         <v>42788</v>
@@ -3229,25 +3223,25 @@
         <v>47</v>
       </c>
       <c r="E56">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56">
-        <v>5.73</v>
+        <v>5.86</v>
       </c>
       <c r="H56" s="1">
         <v>1</v>
       </c>
       <c r="I56" s="1">
-        <v>1.67</v>
+        <v>1.47</v>
       </c>
       <c r="J56" t="s">
         <v>10</v>
       </c>
       <c r="K56">
-        <v>84.89</v>
+        <v>99.65</v>
       </c>
       <c r="L56" t="s">
         <v>63</v>
@@ -3255,10 +3249,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C57" s="2">
         <v>42788</v>
@@ -3267,66 +3261,66 @@
         <v>47</v>
       </c>
       <c r="E57">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
       <c r="G57">
-        <v>6.07</v>
+        <v>5.73</v>
       </c>
       <c r="H57" s="1">
         <v>1</v>
       </c>
       <c r="I57" s="1">
-        <v>1.55</v>
+        <v>1.67</v>
       </c>
       <c r="J57" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="K57">
-        <v>77.260000000000005</v>
+        <v>84.89</v>
       </c>
       <c r="L57" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B58">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C58" s="2">
-        <v>42796</v>
+        <v>42788</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E58">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F58">
         <v>1</v>
       </c>
       <c r="G58">
-        <v>5.52</v>
+        <v>6.07</v>
       </c>
       <c r="H58" s="1">
         <v>1</v>
       </c>
       <c r="I58" s="1">
-        <v>1.57</v>
+        <v>1.55</v>
       </c>
       <c r="J58" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="K58">
-        <v>68.760000000000005</v>
+        <v>77.260000000000005</v>
       </c>
       <c r="L58" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -3352,16 +3346,16 @@
         <v>5.52</v>
       </c>
       <c r="H59" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I59" s="1">
-        <v>1.6</v>
+        <v>1.57</v>
       </c>
       <c r="J59" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="K59">
-        <v>84.89</v>
+        <v>68.760000000000005</v>
       </c>
       <c r="L59" t="s">
         <v>63</v>
@@ -3390,16 +3384,16 @@
         <v>5.52</v>
       </c>
       <c r="H60" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I60" s="1">
         <v>1.6</v>
       </c>
       <c r="J60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K60">
-        <v>92.92</v>
+        <v>84.89</v>
       </c>
       <c r="L60" t="s">
         <v>63</v>
@@ -3407,37 +3401,37 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C61" s="2">
-        <v>42801</v>
+        <v>42796</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E61">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61">
-        <v>5.55</v>
+        <v>5.52</v>
       </c>
       <c r="H61" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I61" s="1">
-        <v>1.66</v>
+        <v>1.6</v>
       </c>
       <c r="J61" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="K61">
-        <v>73.150000000000006</v>
+        <v>92.92</v>
       </c>
       <c r="L61" t="s">
         <v>63</v>
@@ -3460,25 +3454,25 @@
         <v>12</v>
       </c>
       <c r="F62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G62">
-        <v>5.44</v>
+        <v>5.55</v>
       </c>
       <c r="H62" s="1">
         <v>1</v>
       </c>
       <c r="I62" s="1">
-        <v>1.58</v>
+        <v>1.66</v>
       </c>
       <c r="J62" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="K62">
-        <v>77.260000000000005</v>
+        <v>73.150000000000006</v>
       </c>
       <c r="L62" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -3504,16 +3498,16 @@
         <v>5.44</v>
       </c>
       <c r="H63" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I63" s="1">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
       <c r="J63" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K63">
-        <v>87.04</v>
+        <v>77.260000000000005</v>
       </c>
       <c r="L63" t="s">
         <v>106</v>
@@ -3542,16 +3536,16 @@
         <v>5.44</v>
       </c>
       <c r="H64" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I64" s="1">
         <v>1.6</v>
       </c>
       <c r="J64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K64">
-        <v>116.5</v>
+        <v>87.04</v>
       </c>
       <c r="L64" t="s">
         <v>106</v>
@@ -3559,40 +3553,40 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B65">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C65" s="2">
-        <v>42803</v>
+        <v>42801</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>6.67</v>
+        <v>5.44</v>
       </c>
       <c r="H65" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I65" s="1">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="J65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K65">
-        <v>75.56</v>
+        <v>116.5</v>
       </c>
       <c r="L65" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -3618,98 +3612,98 @@
         <v>6.67</v>
       </c>
       <c r="H66" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I66" s="1">
-        <v>1.92</v>
+        <v>1.7</v>
       </c>
       <c r="J66" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K66">
-        <v>83.85</v>
+        <v>75.56</v>
       </c>
       <c r="L66" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67">
+        <v>15</v>
+      </c>
+      <c r="C67" s="2">
+        <v>42803</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>6.67</v>
+      </c>
+      <c r="H67" s="1">
+        <v>2</v>
+      </c>
+      <c r="I67" s="1">
+        <v>1.92</v>
+      </c>
+      <c r="J67" t="s">
+        <v>112</v>
+      </c>
+      <c r="K67">
+        <v>83.85</v>
+      </c>
+      <c r="L67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="B67" s="4">
-        <v>16</v>
-      </c>
-      <c r="C67" s="5">
-        <v>42803</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E67" s="4">
-        <v>3</v>
-      </c>
-      <c r="F67" s="4">
-        <v>1</v>
-      </c>
-      <c r="G67" s="4">
-        <v>6.21</v>
-      </c>
-      <c r="H67" s="6">
-        <v>1</v>
-      </c>
-      <c r="I67" s="6">
-        <v>1.7</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K67" s="4">
-        <v>44.94</v>
-      </c>
-      <c r="L67" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="M67" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="B68" s="4">
         <v>16</v>
       </c>
-      <c r="C68" s="2">
-        <v>42808</v>
+      <c r="C68" s="5">
+        <v>42803</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E68" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F68" s="4">
         <v>1</v>
       </c>
       <c r="G68" s="4">
-        <v>6.47</v>
+        <v>6.21</v>
       </c>
       <c r="H68" s="6">
         <v>1</v>
       </c>
       <c r="I68" s="6">
-        <v>1.68</v>
+        <v>1.7</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="K68" s="4">
-        <v>61.95</v>
+        <v>44.94</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -3735,16 +3729,16 @@
         <v>6.47</v>
       </c>
       <c r="H69" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I69" s="6">
-        <v>1.7</v>
+        <v>1.68</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="K69" s="4">
-        <v>71.63</v>
+        <v>61.95</v>
       </c>
       <c r="L69" s="4" t="s">
         <v>63</v>
@@ -3752,37 +3746,37 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B70" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C70" s="2">
-        <v>42810</v>
+        <v>42808</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E70" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F70" s="4">
         <v>1</v>
       </c>
       <c r="G70" s="4">
-        <v>6.19</v>
+        <v>6.47</v>
       </c>
       <c r="H70" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I70" s="6">
-        <v>1.55</v>
+        <v>1.7</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="K70" s="4">
-        <v>68.760000000000005</v>
+        <v>71.63</v>
       </c>
       <c r="L70" s="4" t="s">
         <v>63</v>
@@ -3811,16 +3805,16 @@
         <v>6.19</v>
       </c>
       <c r="H71" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I71" s="6">
-        <v>1.6</v>
+        <v>1.55</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="K71" s="4">
-        <v>105.8</v>
+        <v>68.760000000000005</v>
       </c>
       <c r="L71" s="4" t="s">
         <v>63</v>
@@ -3849,16 +3843,16 @@
         <v>6.19</v>
       </c>
       <c r="H72" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I72" s="6">
-        <v>1.55</v>
+        <v>1.6</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K72" s="4">
-        <v>71.63</v>
+        <v>105.8</v>
       </c>
       <c r="L72" s="4" t="s">
         <v>63</v>
@@ -3866,10 +3860,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B73" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C73" s="2">
         <v>42810</v>
@@ -3878,25 +3872,25 @@
         <v>47</v>
       </c>
       <c r="E73" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F73" s="4">
         <v>1</v>
       </c>
       <c r="G73" s="4">
-        <v>6.37</v>
+        <v>6.19</v>
       </c>
       <c r="H73" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I73" s="6">
-        <v>1.3</v>
+        <v>1.55</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="K73" s="4">
-        <v>87.84</v>
+        <v>71.63</v>
       </c>
       <c r="L73" s="4" t="s">
         <v>63</v>
@@ -3925,16 +3919,16 @@
         <v>6.37</v>
       </c>
       <c r="H74" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I74" s="6">
         <v>1.3</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="K74" s="4">
-        <v>80.900000000000006</v>
+        <v>87.84</v>
       </c>
       <c r="L74" s="4" t="s">
         <v>63</v>
@@ -3963,16 +3957,16 @@
         <v>6.37</v>
       </c>
       <c r="H75" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I75" s="6">
-        <v>1.58</v>
+        <v>1.3</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K75" s="4">
-        <v>96.85</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="L75" s="4" t="s">
         <v>63</v>
@@ -3980,37 +3974,37 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B76" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C76" s="2">
-        <v>42815</v>
+        <v>42810</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E76" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F76" s="4">
         <v>1</v>
       </c>
       <c r="G76" s="4">
-        <v>4.8099999999999996</v>
+        <v>6.37</v>
       </c>
       <c r="H76" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I76" s="6">
-        <v>1.56</v>
+        <v>1.58</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="K76" s="4">
-        <v>104.2</v>
+        <v>96.85</v>
       </c>
       <c r="L76" s="4" t="s">
         <v>63</v>
@@ -4018,10 +4012,10 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B77" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C77" s="2">
         <v>42815</v>
@@ -4030,28 +4024,28 @@
         <v>47</v>
       </c>
       <c r="E77" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F77" s="4">
         <v>1</v>
       </c>
       <c r="G77" s="4">
-        <v>5.0999999999999996</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="H77" s="6">
         <v>1</v>
       </c>
       <c r="I77" s="6">
-        <v>1.62</v>
+        <v>1.56</v>
       </c>
       <c r="J77" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K77" s="4">
+        <v>104.2</v>
+      </c>
+      <c r="L77" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="K77" s="4">
-        <v>73.94</v>
-      </c>
-      <c r="L77" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -4077,16 +4071,16 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H78" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I78" s="6">
-        <v>1.6</v>
+        <v>1.62</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="K78" s="4">
-        <v>90.48</v>
+        <v>73.94</v>
       </c>
       <c r="L78" s="4" t="s">
         <v>124</v>
@@ -4115,16 +4109,16 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H79" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I79" s="6">
-        <v>1.52</v>
+        <v>1.6</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="K79" s="4">
-        <v>122.8</v>
+        <v>90.48</v>
       </c>
       <c r="L79" s="4" t="s">
         <v>124</v>
@@ -4132,13 +4126,13 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B80" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C80" s="2">
-        <v>42817</v>
+        <v>42815</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>47</v>
@@ -4150,22 +4144,22 @@
         <v>1</v>
       </c>
       <c r="G80" s="4">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H80" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I80" s="6">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="K80" s="4">
-        <v>73.94</v>
+        <v>122.8</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
@@ -4191,16 +4185,16 @@
         <v>5.2</v>
       </c>
       <c r="H81" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I81" s="6">
-        <v>1.31</v>
+        <v>1.5</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="K81" s="4">
-        <v>66.760000000000005</v>
+        <v>73.94</v>
       </c>
       <c r="L81" s="4" t="s">
         <v>63</v>
@@ -4208,10 +4202,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B82" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C82" s="2">
         <v>42817</v>
@@ -4220,66 +4214,66 @@
         <v>47</v>
       </c>
       <c r="E82" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F82" s="4">
         <v>1</v>
       </c>
       <c r="G82" s="4">
-        <v>5.47</v>
+        <v>5.2</v>
       </c>
       <c r="H82" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82" s="6">
-        <v>1.52</v>
+        <v>1.31</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="K82" s="4">
-        <v>63.08</v>
+        <v>66.760000000000005</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B83" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C83" s="2">
-        <v>42821</v>
+        <v>42817</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E83" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F83" s="4">
         <v>1</v>
       </c>
       <c r="G83" s="4">
-        <v>6.53</v>
+        <v>5.47</v>
       </c>
       <c r="H83" s="6">
         <v>1</v>
       </c>
       <c r="I83" s="6">
-        <v>1.72</v>
+        <v>1.52</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="K83" s="4">
-        <v>84.89</v>
+        <v>63.08</v>
       </c>
       <c r="L83" s="4" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
@@ -4305,16 +4299,16 @@
         <v>6.53</v>
       </c>
       <c r="H84" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I84" s="6">
-        <v>1.52</v>
+        <v>1.72</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K84" s="4">
-        <v>68.760000000000005</v>
+        <v>84.89</v>
       </c>
       <c r="L84" s="4" t="s">
         <v>63</v>
@@ -4343,16 +4337,16 @@
         <v>6.53</v>
       </c>
       <c r="H85" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I85" s="6">
-        <v>1.69</v>
+        <v>1.52</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="K85" s="4">
-        <v>78.14</v>
+        <v>68.760000000000005</v>
       </c>
       <c r="L85" s="4" t="s">
         <v>63</v>
@@ -4360,43 +4354,40 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B86" s="4">
         <v>15</v>
       </c>
       <c r="C86" s="2">
-        <v>42822</v>
+        <v>42821</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E86" s="4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F86" s="4">
         <v>1</v>
       </c>
       <c r="G86" s="4">
-        <v>4.66</v>
+        <v>6.53</v>
       </c>
       <c r="H86" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I86" s="6">
-        <v>1.6</v>
+        <v>1.69</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="K86" s="4">
-        <v>73.150000000000006</v>
+        <v>78.14</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M86" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -4422,19 +4413,22 @@
         <v>4.66</v>
       </c>
       <c r="H87" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I87" s="6">
         <v>1.6</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="K87" s="4">
-        <v>77.260000000000005</v>
+        <v>73.150000000000006</v>
       </c>
       <c r="L87" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="M87" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -4460,16 +4454,16 @@
         <v>4.66</v>
       </c>
       <c r="H88" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I88" s="6">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K88" s="4">
-        <v>74.739999999999995</v>
+        <v>77.260000000000005</v>
       </c>
       <c r="L88" s="4" t="s">
         <v>19</v>
@@ -4498,16 +4492,16 @@
         <v>4.66</v>
       </c>
       <c r="H89" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I89" s="6">
         <v>1.2</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K89" s="4">
-        <v>72.38</v>
+        <v>74.739999999999995</v>
       </c>
       <c r="L89" s="4" t="s">
         <v>19</v>
@@ -4515,10 +4509,10 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B90" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C90" s="2">
         <v>42822</v>
@@ -4527,28 +4521,28 @@
         <v>47</v>
       </c>
       <c r="E90" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F90" s="4">
         <v>1</v>
       </c>
       <c r="G90" s="4">
-        <v>5.16</v>
+        <v>4.66</v>
       </c>
       <c r="H90" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I90" s="6">
-        <v>1.57</v>
+        <v>1.2</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="K90" s="4">
-        <v>88.16</v>
+        <v>72.38</v>
       </c>
       <c r="L90" s="4" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -4574,16 +4568,16 @@
         <v>5.16</v>
       </c>
       <c r="H91" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I91" s="6">
-        <v>1.3</v>
+        <v>1.57</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="K91" s="4">
-        <v>96.85</v>
+        <v>88.16</v>
       </c>
       <c r="L91" s="4" t="s">
         <v>58</v>
@@ -4591,40 +4585,40 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B92" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C92" s="2">
-        <v>42824</v>
+        <v>42822</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E92" s="4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F92" s="4">
         <v>1</v>
       </c>
       <c r="G92" s="4">
-        <v>7.43</v>
+        <v>5.16</v>
       </c>
       <c r="H92" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I92" s="6">
-        <v>1.77</v>
+        <v>1.3</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="K92" s="4">
-        <v>41.47</v>
+        <v>96.85</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -4650,16 +4644,16 @@
         <v>7.43</v>
       </c>
       <c r="H93" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I93" s="6">
-        <v>1.8</v>
+        <v>1.77</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="K93" s="4">
-        <v>75.56</v>
+        <v>41.47</v>
       </c>
       <c r="L93" s="4" t="s">
         <v>19</v>
@@ -4688,16 +4682,16 @@
         <v>7.43</v>
       </c>
       <c r="H94" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I94" s="6">
-        <v>1.83</v>
+        <v>1.8</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K94" s="4">
-        <v>45.24</v>
+        <v>75.56</v>
       </c>
       <c r="L94" s="4" t="s">
         <v>19</v>
@@ -4705,40 +4699,40 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B95" s="4">
         <v>15</v>
       </c>
       <c r="C95" s="2">
-        <v>42828</v>
+        <v>42824</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E95" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" s="4">
         <v>1</v>
       </c>
       <c r="G95" s="4">
-        <v>6.29</v>
+        <v>7.43</v>
       </c>
       <c r="H95" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I95" s="6">
-        <v>1.64</v>
+        <v>1.83</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="K95" s="4">
-        <v>72.38</v>
+        <v>45.24</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -4764,16 +4758,16 @@
         <v>6.29</v>
       </c>
       <c r="H96" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I96" s="6">
-        <v>1.54</v>
+        <v>1.64</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="K96" s="4">
-        <v>80.900000000000006</v>
+        <v>72.38</v>
       </c>
       <c r="L96" s="4" t="s">
         <v>63</v>
@@ -4802,16 +4796,16 @@
         <v>6.29</v>
       </c>
       <c r="H97" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I97" s="6">
-        <v>1.64</v>
+        <v>1.54</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K97" s="4">
-        <v>68.08</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="L97" s="4" t="s">
         <v>63</v>
@@ -4840,16 +4834,16 @@
         <v>6.29</v>
       </c>
       <c r="H98" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I98" s="6">
-        <v>1.58</v>
+        <v>1.64</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K98" s="4">
-        <v>95.5</v>
+        <v>68.08</v>
       </c>
       <c r="L98" s="4" t="s">
         <v>63</v>
@@ -4878,16 +4872,16 @@
         <v>6.29</v>
       </c>
       <c r="H99" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I99" s="6">
         <v>1.58</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K99" s="4">
-        <v>66.760000000000005</v>
+        <v>95.5</v>
       </c>
       <c r="L99" s="4" t="s">
         <v>63</v>
@@ -4895,40 +4889,40 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B100" s="4">
         <v>15</v>
       </c>
       <c r="C100" s="2">
-        <v>42829</v>
+        <v>42828</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E100" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F100" s="4">
         <v>1</v>
       </c>
-      <c r="G100" s="3">
-        <v>6.23</v>
+      <c r="G100" s="4">
+        <v>6.29</v>
       </c>
       <c r="H100" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I100" s="6">
-        <v>1.35</v>
+        <v>1.58</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="K100" s="4">
-        <v>72.38</v>
+        <v>66.760000000000005</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
@@ -4954,16 +4948,16 @@
         <v>6.23</v>
       </c>
       <c r="H101" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I101" s="6">
-        <v>1.61</v>
+        <v>1.35</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="K101" s="4">
-        <v>67.41</v>
+        <v>72.38</v>
       </c>
       <c r="L101" s="4" t="s">
         <v>19</v>
@@ -4992,16 +4986,16 @@
         <v>6.23</v>
       </c>
       <c r="H102" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I102" s="6">
-        <v>1.35</v>
+        <v>1.61</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="K102" s="4">
-        <v>70.89</v>
+        <v>67.41</v>
       </c>
       <c r="L102" s="4" t="s">
         <v>19</v>
@@ -5024,58 +5018,138 @@
         <v>7</v>
       </c>
       <c r="F103" s="4">
+        <v>1</v>
+      </c>
+      <c r="G103" s="3">
+        <v>6.23</v>
+      </c>
+      <c r="H103" s="6">
+        <v>3</v>
+      </c>
+      <c r="I103" s="6">
+        <v>1.35</v>
+      </c>
+      <c r="J103" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K103" s="4">
+        <v>70.89</v>
+      </c>
+      <c r="L103" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B104" s="4">
+        <v>15</v>
+      </c>
+      <c r="C104" s="2">
+        <v>42829</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E104" s="4">
+        <v>7</v>
+      </c>
+      <c r="F104" s="4">
         <v>2</v>
       </c>
-      <c r="G103" s="3">
+      <c r="G104" s="3">
         <v>5.59</v>
       </c>
-      <c r="H103" s="6">
-        <v>1</v>
-      </c>
-      <c r="I103" s="6">
+      <c r="H104" s="6">
+        <v>1</v>
+      </c>
+      <c r="I104" s="6">
         <v>1.4</v>
       </c>
-      <c r="J103" s="4" t="s">
+      <c r="J104" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K103" s="4">
+      <c r="K104" s="4">
         <v>98.23</v>
-      </c>
-      <c r="L103" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H104" s="6">
-        <v>2</v>
-      </c>
-      <c r="I104" s="6">
-        <v>1.48</v>
-      </c>
-      <c r="J104" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K104" s="4">
-        <v>50.19</v>
       </c>
       <c r="L104" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B105" s="4">
+        <v>15</v>
+      </c>
+      <c r="C105" s="2">
+        <v>42829</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E105" s="4">
+        <v>7</v>
+      </c>
+      <c r="F105" s="4">
+        <v>2</v>
+      </c>
+      <c r="G105" s="3">
+        <v>5.59</v>
+      </c>
       <c r="H105" s="6">
+        <v>2</v>
+      </c>
+      <c r="I105" s="6">
+        <v>1.48</v>
+      </c>
+      <c r="J105" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K105" s="4">
+        <v>50.19</v>
+      </c>
+      <c r="L105" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B106" s="4">
+        <v>15</v>
+      </c>
+      <c r="C106" s="2">
+        <v>42829</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E106" s="4">
+        <v>7</v>
+      </c>
+      <c r="F106" s="4">
+        <v>2</v>
+      </c>
+      <c r="G106" s="3">
+        <v>5.59</v>
+      </c>
+      <c r="H106" s="6">
         <v>3</v>
       </c>
-      <c r="I105" s="6">
+      <c r="I106" s="6">
         <v>1.6</v>
       </c>
-      <c r="J105" s="4" t="s">
+      <c r="J106" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K105" s="4">
+      <c r="K106" s="4">
         <v>81.86</v>
       </c>
-      <c r="L105" s="4" t="s">
+      <c r="L106" s="4" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>